<commit_message>
Identificação de novos metabolitos
</commit_message>
<xml_diff>
--- a/regioes_integrais.xlsx
+++ b/regioes_integrais.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorj\Documents\Edmilson\Analise_sururu_preto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edmil\Documents\Analise_sururu_preto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03739CF9-CA75-4798-B2BD-78B8B1E7A2F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C90A16-F2F7-4787-8444-7C086259583D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40455" yWindow="4395" windowWidth="16200" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Metabolito</t>
   </si>
@@ -46,6 +46,66 @@
   </si>
   <si>
     <t>Propionic acid</t>
+  </si>
+  <si>
+    <t>Lactate</t>
+  </si>
+  <si>
+    <t>Alanine</t>
+  </si>
+  <si>
+    <t>Unknow</t>
+  </si>
+  <si>
+    <t>Unknow_1</t>
+  </si>
+  <si>
+    <t>Unknow_2</t>
+  </si>
+  <si>
+    <t>Unknow_3</t>
+  </si>
+  <si>
+    <t>2-Aminoisobutyric acid</t>
+  </si>
+  <si>
+    <t>Unknow_4</t>
+  </si>
+  <si>
+    <t>L-arginine/Leucine</t>
+  </si>
+  <si>
+    <t>Unknow_5</t>
+  </si>
+  <si>
+    <t>Unknow_6</t>
+  </si>
+  <si>
+    <t>Acetate</t>
+  </si>
+  <si>
+    <t>Acetylphosphate</t>
+  </si>
+  <si>
+    <t>Homoserine</t>
+  </si>
+  <si>
+    <t>Acetylglycine</t>
+  </si>
+  <si>
+    <t>Acetylcysteine</t>
+  </si>
+  <si>
+    <t>Acetylcholine</t>
+  </si>
+  <si>
+    <t>Acetone/3-hidroxybutyrate</t>
+  </si>
+  <si>
+    <t>Piruvate</t>
+  </si>
+  <si>
+    <t>Beta-alanine</t>
   </si>
 </sst>
 </file>
@@ -363,15 +423,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,7 +445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -393,7 +456,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -404,7 +467,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -415,7 +478,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -424,6 +487,226 @@
       </c>
       <c r="C5">
         <v>1.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1.32</v>
+      </c>
+      <c r="C6">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>1.3680000000000001</v>
+      </c>
+      <c r="C7">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1.38</v>
+      </c>
+      <c r="C8">
+        <v>1.405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>1.425</v>
+      </c>
+      <c r="C9">
+        <v>1.4350000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1.4650000000000001</v>
+      </c>
+      <c r="C10">
+        <v>1.5049999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1.5</v>
+      </c>
+      <c r="C11">
+        <v>1.5149999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>1.5149999999999999</v>
+      </c>
+      <c r="C12">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>1.66</v>
+      </c>
+      <c r="C13">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>1.81</v>
+      </c>
+      <c r="C14">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>1.865</v>
+      </c>
+      <c r="C15">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>1.893</v>
+      </c>
+      <c r="C16">
+        <v>1.915</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>1.915</v>
+      </c>
+      <c r="C17">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>1.98</v>
+      </c>
+      <c r="C18">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="C19">
+        <v>2.0649999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>2.0659999999999998</v>
+      </c>
+      <c r="C20">
+        <v>2.077</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>2.13</v>
+      </c>
+      <c r="C21">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>2.2349999999999999</v>
+      </c>
+      <c r="C22">
+        <v>2.3050000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>2.4</v>
+      </c>
+      <c r="C23">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="C24">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="C25">
+        <v>2.585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Analises do sururu para a apresentação de seminarios
</commit_message>
<xml_diff>
--- a/regioes_integrais.xlsx
+++ b/regioes_integrais.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edmil\Documents\Analise_sururu_preto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorj\Documents\Edmilson\Analise_sururu_preto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C90A16-F2F7-4787-8444-7C086259583D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D380B476-02A4-4A97-ADA9-84EBE7E54AF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Metabolito</t>
   </si>
@@ -106,6 +106,60 @@
   </si>
   <si>
     <t>Beta-alanine</t>
+  </si>
+  <si>
+    <t>Methyluric acid</t>
+  </si>
+  <si>
+    <t>Dimethylsulfone</t>
+  </si>
+  <si>
+    <t>Dimethylxantine</t>
+  </si>
+  <si>
+    <t>3-Methylhistidine</t>
+  </si>
+  <si>
+    <t>Adenosine</t>
+  </si>
+  <si>
+    <t>FADH</t>
+  </si>
+  <si>
+    <t>Unknow_7</t>
+  </si>
+  <si>
+    <t>Inosine</t>
+  </si>
+  <si>
+    <t>Choline</t>
+  </si>
+  <si>
+    <t>Aspartate</t>
+  </si>
+  <si>
+    <t>Tirosine</t>
+  </si>
+  <si>
+    <t>Beta-leucine</t>
+  </si>
+  <si>
+    <t>Methylhistidine</t>
+  </si>
+  <si>
+    <t>Phenylalanine</t>
+  </si>
+  <si>
+    <t>Deoxyinosine</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>Histamine</t>
+  </si>
+  <si>
+    <t>Inosine_2</t>
   </si>
 </sst>
 </file>
@@ -423,18 +477,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,271 +499,472 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>1.5</v>
+      </c>
+      <c r="C2">
+        <v>1.5149999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>7.92</v>
+      </c>
+      <c r="C3">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>1.893</v>
+      </c>
+      <c r="C4">
+        <v>1.915</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>2.2349999999999999</v>
+      </c>
+      <c r="C5">
+        <v>2.3050000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>2.13</v>
+      </c>
+      <c r="C6">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>2.0659999999999998</v>
+      </c>
+      <c r="C7">
+        <v>2.077</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>2.04</v>
+      </c>
+      <c r="C8">
+        <v>2.0649999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>1.915</v>
+      </c>
+      <c r="C9">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>8.2449999999999992</v>
+      </c>
+      <c r="C10">
+        <v>8.2750000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>8.58</v>
+      </c>
+      <c r="C11">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>1.4650000000000001</v>
+      </c>
+      <c r="C12">
+        <v>1.5049999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>2.68</v>
+      </c>
+      <c r="C13">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="C14">
+        <v>2.585</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>3.32</v>
+      </c>
+      <c r="C15">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>4.04</v>
+      </c>
+      <c r="C16">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17">
+        <v>6.48</v>
+      </c>
+      <c r="C17">
+        <v>6.52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>3.13</v>
+      </c>
+      <c r="C18">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19">
+        <v>3.35</v>
+      </c>
+      <c r="C19">
+        <v>3.3650000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>5.7949999999999999</v>
+      </c>
+      <c r="C20">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21">
+        <v>7.8949999999999996</v>
+      </c>
+      <c r="C21">
+        <v>7.923</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>1.98</v>
+      </c>
+      <c r="C22">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>6.0919999999999996</v>
+      </c>
+      <c r="C23">
+        <v>6.13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24">
+        <v>8.34</v>
+      </c>
+      <c r="C24">
+        <v>8.3699999999999992</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B25">
         <v>0.92</v>
       </c>
-      <c r="C2">
+      <c r="C25">
         <v>0.95</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>1.32</v>
+      </c>
+      <c r="C26">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>1.66</v>
+      </c>
+      <c r="C27">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B28">
         <v>0.95</v>
       </c>
-      <c r="C3">
+      <c r="C28">
         <v>0.98</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29">
+        <v>7.69</v>
+      </c>
+      <c r="C29">
+        <v>7.7110000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>3.25</v>
+      </c>
+      <c r="C30">
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>7.3</v>
+      </c>
+      <c r="C31">
+        <v>7.45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32">
+        <v>2.4</v>
+      </c>
+      <c r="C32">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>1.06</v>
+      </c>
+      <c r="C33">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>6.88</v>
+      </c>
+      <c r="C34">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="C35">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36">
+        <v>1.3680000000000001</v>
+      </c>
+      <c r="C36">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>1.38</v>
+      </c>
+      <c r="C37">
+        <v>1.405</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38">
+        <v>1.425</v>
+      </c>
+      <c r="C38">
+        <v>1.4350000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <v>1.5149999999999999</v>
+      </c>
+      <c r="C39">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40">
+        <v>1.81</v>
+      </c>
+      <c r="C40">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41">
+        <v>1.865</v>
+      </c>
+      <c r="C41">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42">
+        <v>0.75</v>
+      </c>
+      <c r="C42">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B43">
         <v>1.03</v>
       </c>
-      <c r="C4">
+      <c r="C43">
         <v>1.06</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>1.06</v>
-      </c>
-      <c r="C5">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>1.32</v>
-      </c>
-      <c r="C6">
-        <v>1.36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>1.3680000000000001</v>
-      </c>
-      <c r="C7">
-        <v>1.38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>1.38</v>
-      </c>
-      <c r="C8">
-        <v>1.405</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>1.425</v>
-      </c>
-      <c r="C9">
-        <v>1.4350000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1.4650000000000001</v>
-      </c>
-      <c r="C10">
-        <v>1.5049999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>1.5</v>
-      </c>
-      <c r="C11">
-        <v>1.5149999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>1.5149999999999999</v>
-      </c>
-      <c r="C12">
-        <v>1.53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
-        <v>1.66</v>
-      </c>
-      <c r="C13">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14">
-        <v>1.81</v>
-      </c>
-      <c r="C14">
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>1.865</v>
-      </c>
-      <c r="C15">
-        <v>1.88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>1.893</v>
-      </c>
-      <c r="C16">
-        <v>1.915</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>1.915</v>
-      </c>
-      <c r="C17">
-        <v>1.94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>1.98</v>
-      </c>
-      <c r="C18">
-        <v>2.0299999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="C19">
-        <v>2.0649999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20">
-        <v>2.0659999999999998</v>
-      </c>
-      <c r="C20">
-        <v>2.077</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21">
-        <v>2.13</v>
-      </c>
-      <c r="C21">
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22">
-        <v>2.2349999999999999</v>
-      </c>
-      <c r="C22">
-        <v>2.3050000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23">
-        <v>2.4</v>
-      </c>
-      <c r="C23">
-        <v>2.42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="C24">
-        <v>2.54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="C25">
-        <v>2.585</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C43">
+    <sortCondition ref="A1:A43"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>